<commit_message>
Updated May training plan
</commit_message>
<xml_diff>
--- a/blog/posts/MayProgram/data/May.xlsx
+++ b/blog/posts/MayProgram/data/May.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/edwardcr_qut_edu_au/Documents/Research/_website/edwchris.github.io/blog/posts/MayProgram/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{47611721-5055-4085-82E7-0FAFA3913107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBA65AEC-2571-408E-81A9-2935FBF86D1B}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{47611721-5055-4085-82E7-0FAFA3913107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABB57084-34E1-47ED-B560-6CE005CE7DA4}"/>
   <bookViews>
-    <workbookView xWindow="-50" yWindow="0" windowWidth="36730" windowHeight="20880" xr2:uid="{91CA0F68-18E3-4C81-872C-2247EA87DE44}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="25420" windowHeight="13920" xr2:uid="{91CA0F68-18E3-4C81-872C-2247EA87DE44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>1:25 hours easy to HR</t>
   </si>
   <si>
-    <t>1:30 hours easy to HR</t>
-  </si>
-  <si>
     <t>1:35 hours easy to HR</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>30k with 3 x 4k at MP plus 2k at HMP (last effort)</t>
   </si>
   <si>
-    <t>Rest</t>
-  </si>
-  <si>
     <t>2:20 hours easy to HR</t>
   </si>
   <si>
@@ -128,10 +122,16 @@
     <t>Watts thresholds with longer WU and WD (say 4k each)</t>
   </si>
   <si>
-    <t>10k easy to HR with 1k at HMP or Watts pre-Noosa Thursday session</t>
-  </si>
-  <si>
-    <t>Gym (easy)</t>
+    <t xml:space="preserve">10k easy to HR with 2 x 500m at HMP </t>
+  </si>
+  <si>
+    <t>Rest day or 30min very slow jog</t>
+  </si>
+  <si>
+    <t>5k easy with 6 to 8 100m efforts to 4:05 pace.</t>
+  </si>
+  <si>
+    <t>10km easy</t>
   </si>
 </sst>
 </file>
@@ -514,7 +514,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -563,22 +563,22 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -589,7 +589,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
@@ -601,10 +601,10 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -615,22 +615,22 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
       <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
         <v>30</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
         <v>31</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -641,13 +641,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
         <v>4</v>
@@ -656,7 +656,7 @@
         <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>